<commit_message>
Update merged test file.
</commit_message>
<xml_diff>
--- a/tests/files/input-merged.xlsx
+++ b/tests/files/input-merged.xlsx
@@ -34,10 +34,10 @@
     <t xml:space="preserve">Organización</t>
   </si>
   <si>
+    <t xml:space="preserve">Mujeres</t>
+  </si>
+  <si>
     <t xml:space="preserve">Hombres</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mujeres</t>
   </si>
   <si>
     <t xml:space="preserve">País</t>
@@ -334,7 +334,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="bottomLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>